<commit_message>
data structure altered to package each data point calculation into a single json response (height/weight/bmi/ofc as separate responses). Added facility for charting multiple data points on a single child
</commit_message>
<xml_diff>
--- a/static/uploaded_data/dummy_data.xlsx
+++ b/static/uploaded_data/dummy_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SimonChapman/Desktop/RCPCH Growth Chart Reference Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81F3C0B-684C-5D47-8E8B-7CE83740CF5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4064639-B619-684A-89D2-15D2592940AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{223B1396-2B9F-8546-98EB-3EE280CD9F37}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16320" xr2:uid="{223B1396-2B9F-8546-98EB-3EE280CD9F37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="11">
   <si>
     <t>measurement_value</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>sex</t>
-  </si>
-  <si>
-    <t>decimal_age</t>
-  </si>
-  <si>
-    <t>estimated_date_delivery</t>
   </si>
   <si>
     <t>gestation_days</t>
@@ -427,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C34F8A-12E7-3A49-9B1D-BA3C1E2BC243}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,42 +433,34 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>40515</v>
       </c>
@@ -484,23 +470,17 @@
       <c r="C2">
         <v>27</v>
       </c>
-      <c r="E2" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F2">
-        <v>-0.24914442162902101</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2">
         <v>1.21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>40515</v>
       </c>
@@ -510,23 +490,17 @@
       <c r="C3">
         <v>27</v>
       </c>
-      <c r="E3" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F3">
-        <v>-0.20260095824777599</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3">
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>40515</v>
       </c>
@@ -536,23 +510,17 @@
       <c r="C4">
         <v>27</v>
       </c>
-      <c r="E4" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F4">
-        <v>1.01300479123888</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4">
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>40515</v>
       </c>
@@ -562,23 +530,17 @@
       <c r="C5">
         <v>27</v>
       </c>
-      <c r="E5" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F5">
-        <v>1.3032169746748801</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
         <v>84.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>40515</v>
       </c>
@@ -588,23 +550,17 @@
       <c r="C6">
         <v>27</v>
       </c>
-      <c r="E6" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F6">
-        <v>3.9835728952772098</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6">
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
         <v>100.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>38177</v>
       </c>
@@ -614,23 +570,17 @@
       <c r="C7">
         <v>35</v>
       </c>
-      <c r="E7" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F7">
-        <v>0.161533196440794</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7">
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
         <v>4.17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>38177</v>
       </c>
@@ -640,23 +590,17 @@
       <c r="C8">
         <v>35</v>
       </c>
-      <c r="E8" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F8">
-        <v>0.161533196440794</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
         <v>54.8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>39904</v>
       </c>
@@ -666,20 +610,17 @@
       <c r="C9">
         <v>40</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9">
         <v>2.7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>39904</v>
       </c>
@@ -689,20 +630,17 @@
       <c r="C10">
         <v>40</v>
       </c>
-      <c r="F10">
-        <v>0.25188227241615302</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10">
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
         <v>4.57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>39904</v>
       </c>
@@ -712,20 +650,17 @@
       <c r="C11">
         <v>40</v>
       </c>
-      <c r="F11">
-        <v>0.30390143737166297</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11">
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>39904</v>
       </c>
@@ -735,20 +670,17 @@
       <c r="C12">
         <v>40</v>
       </c>
-      <c r="F12">
-        <v>0.30390143737166297</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12">
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>39904</v>
       </c>
@@ -758,20 +690,17 @@
       <c r="C13">
         <v>40</v>
       </c>
-      <c r="F13">
-        <v>0.323066392881588</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13">
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>40515</v>
       </c>
@@ -781,23 +710,17 @@
       <c r="C14">
         <v>27</v>
       </c>
-      <c r="E14" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F14">
-        <v>0.33127994524298399</v>
-      </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14">
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>40515</v>
       </c>
@@ -807,23 +730,17 @@
       <c r="C15">
         <v>27</v>
       </c>
-      <c r="E15" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F15">
-        <v>0.89527720739219696</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15">
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15">
         <v>10.7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>40515</v>
       </c>
@@ -833,23 +750,17 @@
       <c r="C16">
         <v>27</v>
       </c>
-      <c r="E16" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F16">
-        <v>2.2888432580424398</v>
-      </c>
-      <c r="G16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16">
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16">
         <v>12.4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>40515</v>
       </c>
@@ -859,23 +770,17 @@
       <c r="C17">
         <v>27</v>
       </c>
-      <c r="E17" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F17">
-        <v>2.5872689938398401</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17">
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17">
         <v>12.5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>40515</v>
       </c>
@@ -885,23 +790,17 @@
       <c r="C18">
         <v>27</v>
       </c>
-      <c r="E18" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F18">
-        <v>3.2717316906228602</v>
-      </c>
-      <c r="G18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18">
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18">
         <v>13.8</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>40515</v>
       </c>
@@ -911,23 +810,17 @@
       <c r="C19">
         <v>27</v>
       </c>
-      <c r="E19" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F19">
-        <v>3.5044490075290899</v>
-      </c>
-      <c r="G19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19">
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19">
         <v>13.6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>40515</v>
       </c>
@@ -937,23 +830,17 @@
       <c r="C20">
         <v>27</v>
       </c>
-      <c r="E20" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F20">
-        <v>3.8083504449007499</v>
-      </c>
-      <c r="G20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20">
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20">
         <v>14.1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>40515</v>
       </c>
@@ -963,23 +850,17 @@
       <c r="C21">
         <v>27</v>
       </c>
-      <c r="E21" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F21">
-        <v>4.4626967830253204</v>
-      </c>
-      <c r="G21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21">
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21">
         <v>15.36</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>40515</v>
       </c>
@@ -989,23 +870,17 @@
       <c r="C22">
         <v>27</v>
       </c>
-      <c r="E22" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F22">
-        <v>1.01300479123888</v>
-      </c>
-      <c r="G22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22">
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>40515</v>
       </c>
@@ -1015,23 +890,17 @@
       <c r="C23">
         <v>27</v>
       </c>
-      <c r="E23" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F23">
-        <v>3.2717316906228602</v>
-      </c>
-      <c r="G23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" t="s">
-        <v>12</v>
-      </c>
-      <c r="I23">
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>40515</v>
       </c>
@@ -1041,23 +910,17 @@
       <c r="C24">
         <v>27</v>
       </c>
-      <c r="E24" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F24">
-        <v>3.5044490075290899</v>
-      </c>
-      <c r="G24" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24">
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>40515</v>
       </c>
@@ -1067,23 +930,17 @@
       <c r="C25">
         <v>27</v>
       </c>
-      <c r="E25" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F25">
-        <v>3.8083504449007499</v>
-      </c>
-      <c r="G25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25">
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25">
         <v>99.5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>40515</v>
       </c>
@@ -1093,23 +950,17 @@
       <c r="C26">
         <v>27</v>
       </c>
-      <c r="E26" s="2">
-        <v>40606</v>
-      </c>
-      <c r="F26">
-        <v>4.4626967830253204</v>
-      </c>
-      <c r="G26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26">
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26">
         <v>100.8</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>38177</v>
       </c>
@@ -1119,23 +970,17 @@
       <c r="C27">
         <v>35</v>
       </c>
-      <c r="E27" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F27">
-        <v>-9.5824777549623499E-2</v>
-      </c>
-      <c r="G27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27">
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27">
         <v>3.09</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>38177</v>
       </c>
@@ -1145,23 +990,17 @@
       <c r="C28">
         <v>35</v>
       </c>
-      <c r="E28" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F28">
-        <v>0.396988364134155</v>
-      </c>
-      <c r="G28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28">
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28">
         <v>5.23</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>38177</v>
       </c>
@@ -1171,23 +1010,17 @@
       <c r="C29">
         <v>35</v>
       </c>
-      <c r="E29" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F29">
-        <v>0.79397672826830901</v>
-      </c>
-      <c r="G29" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29">
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29">
         <v>5.85</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>38177</v>
       </c>
@@ -1197,23 +1030,17 @@
       <c r="C30">
         <v>35</v>
       </c>
-      <c r="E30" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F30">
-        <v>1.0650239561943899</v>
-      </c>
-      <c r="G30" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30">
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30">
         <v>6.62</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>38177</v>
       </c>
@@ -1223,23 +1050,17 @@
       <c r="C31">
         <v>35</v>
       </c>
-      <c r="E31" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F31">
-        <v>1.3305954825462001</v>
-      </c>
-      <c r="G31" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31">
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31">
         <v>7.41</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>38177</v>
       </c>
@@ -1249,23 +1070,17 @@
       <c r="C32">
         <v>35</v>
       </c>
-      <c r="E32" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F32">
-        <v>1.4921286789870001</v>
-      </c>
-      <c r="G32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32">
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32">
         <v>7.25</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>38177</v>
       </c>
@@ -1275,23 +1090,17 @@
       <c r="C33">
         <v>35</v>
       </c>
-      <c r="E33" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F33">
-        <v>2.2806297056810401</v>
-      </c>
-      <c r="G33" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33">
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33">
         <v>9.9600000000000009</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>38177</v>
       </c>
@@ -1301,23 +1110,17 @@
       <c r="C34">
         <v>35</v>
       </c>
-      <c r="E34" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F34">
-        <v>2.56536618754278</v>
-      </c>
-      <c r="G34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34">
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34">
         <v>10.84</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>38177</v>
       </c>
@@ -1327,23 +1130,17 @@
       <c r="C35">
         <v>35</v>
       </c>
-      <c r="E35" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F35">
-        <v>0.396988364134155</v>
-      </c>
-      <c r="G35" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" t="s">
-        <v>12</v>
-      </c>
-      <c r="I35">
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35">
         <v>61.7</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>38177</v>
       </c>
@@ -1353,23 +1150,17 @@
       <c r="C36">
         <v>35</v>
       </c>
-      <c r="E36" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F36">
-        <v>0.79397672826830901</v>
-      </c>
-      <c r="G36" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36">
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>38177</v>
       </c>
@@ -1379,23 +1170,17 @@
       <c r="C37">
         <v>35</v>
       </c>
-      <c r="E37" s="2">
-        <v>38212</v>
-      </c>
-      <c r="F37">
-        <v>1.0650239561943899</v>
-      </c>
-      <c r="G37" t="s">
-        <v>10</v>
-      </c>
-      <c r="H37" t="s">
-        <v>12</v>
-      </c>
-      <c r="I37">
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37">
         <v>68.2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>39904</v>
       </c>
@@ -1405,20 +1190,17 @@
       <c r="C38">
         <v>40</v>
       </c>
-      <c r="F38">
-        <v>0.323066392881588</v>
-      </c>
-      <c r="G38" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38">
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38">
         <v>4.67</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>39904</v>
       </c>
@@ -1428,20 +1210,17 @@
       <c r="C39">
         <v>40</v>
       </c>
-      <c r="F39">
-        <v>0.38056125941136199</v>
-      </c>
-      <c r="G39" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39">
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39">
         <v>5.42</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39904</v>
       </c>
@@ -1451,20 +1230,17 @@
       <c r="C40">
         <v>40</v>
       </c>
-      <c r="F40">
-        <v>0.41889117043121099</v>
-      </c>
-      <c r="G40" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40">
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40">
         <v>5.63</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39904</v>
       </c>
@@ -1474,20 +1250,17 @@
       <c r="C41">
         <v>40</v>
       </c>
-      <c r="F41">
-        <v>0.67624914442162898</v>
-      </c>
-      <c r="G41" t="s">
-        <v>9</v>
-      </c>
-      <c r="H41" t="s">
-        <v>11</v>
-      </c>
-      <c r="I41">
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41">
         <v>6.3</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>39904</v>
       </c>
@@ -1497,20 +1270,17 @@
       <c r="C42">
         <v>40</v>
       </c>
-      <c r="F42">
-        <v>0.88706365503080098</v>
-      </c>
-      <c r="G42" t="s">
-        <v>9</v>
-      </c>
-      <c r="H42" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42">
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42">
         <v>7.1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>39904</v>
       </c>
@@ -1520,20 +1290,17 @@
       <c r="C43">
         <v>40</v>
       </c>
-      <c r="F43">
-        <v>0.89801505817932903</v>
-      </c>
-      <c r="G43" t="s">
-        <v>9</v>
-      </c>
-      <c r="H43" t="s">
-        <v>11</v>
-      </c>
-      <c r="I43">
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43">
         <v>7.1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>39904</v>
       </c>
@@ -1543,20 +1310,17 @@
       <c r="C44">
         <v>40</v>
       </c>
-      <c r="F44">
-        <v>1.09514031485284</v>
-      </c>
-      <c r="G44" t="s">
-        <v>9</v>
-      </c>
-      <c r="H44" t="s">
-        <v>11</v>
-      </c>
-      <c r="I44">
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44">
         <v>7.26</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>39904</v>
       </c>
@@ -1566,20 +1330,17 @@
       <c r="C45">
         <v>40</v>
       </c>
-      <c r="F45">
-        <v>1.4592744695414099</v>
-      </c>
-      <c r="G45" t="s">
-        <v>9</v>
-      </c>
-      <c r="H45" t="s">
-        <v>11</v>
-      </c>
-      <c r="I45">
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45">
         <v>8.08</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>39904</v>
       </c>
@@ -1589,20 +1350,17 @@
       <c r="C46">
         <v>40</v>
       </c>
-      <c r="F46">
-        <v>1.5359342915811101</v>
-      </c>
-      <c r="G46" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" t="s">
-        <v>11</v>
-      </c>
-      <c r="I46">
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46">
         <v>8.11</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>39904</v>
       </c>
@@ -1612,20 +1370,17 @@
       <c r="C47">
         <v>40</v>
       </c>
-      <c r="F47">
-        <v>1.7084188911704301</v>
-      </c>
-      <c r="G47" t="s">
-        <v>9</v>
-      </c>
-      <c r="H47" t="s">
-        <v>11</v>
-      </c>
-      <c r="I47">
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47">
         <v>8.1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>39904</v>
       </c>
@@ -1635,20 +1390,17 @@
       <c r="C48">
         <v>40</v>
       </c>
-      <c r="F48">
-        <v>1.9192334017796</v>
-      </c>
-      <c r="G48" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48" t="s">
-        <v>11</v>
-      </c>
-      <c r="I48">
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48">
         <v>8.98</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>39904</v>
       </c>
@@ -1658,20 +1410,17 @@
       <c r="C49">
         <v>40</v>
       </c>
-      <c r="F49">
-        <v>0.38056125941136199</v>
-      </c>
-      <c r="G49" t="s">
-        <v>9</v>
-      </c>
-      <c r="H49" t="s">
-        <v>12</v>
-      </c>
-      <c r="I49">
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>39904</v>
       </c>
@@ -1681,20 +1430,17 @@
       <c r="C50">
         <v>40</v>
       </c>
-      <c r="F50">
-        <v>0.67624914442162898</v>
-      </c>
-      <c r="G50" t="s">
-        <v>9</v>
-      </c>
-      <c r="H50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I50">
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50">
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>39904</v>
       </c>
@@ -1704,20 +1450,17 @@
       <c r="C51">
         <v>40</v>
       </c>
-      <c r="F51">
-        <v>0.88706365503080098</v>
-      </c>
-      <c r="G51" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" t="s">
-        <v>12</v>
-      </c>
-      <c r="I51">
+      <c r="E51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51">
         <v>70.5</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>39904</v>
       </c>
@@ -1727,20 +1470,17 @@
       <c r="C52">
         <v>40</v>
       </c>
-      <c r="F52">
-        <v>1.09514031485284</v>
-      </c>
-      <c r="G52" t="s">
-        <v>9</v>
-      </c>
-      <c r="H52" t="s">
-        <v>12</v>
-      </c>
-      <c r="I52">
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52">
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>39904</v>
       </c>
@@ -1750,20 +1490,17 @@
       <c r="C53">
         <v>40</v>
       </c>
-      <c r="F53">
-        <v>1.4592744695414099</v>
-      </c>
-      <c r="G53" t="s">
-        <v>9</v>
-      </c>
-      <c r="H53" t="s">
-        <v>12</v>
-      </c>
-      <c r="I53">
+      <c r="E53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53">
         <v>75.900000000000006</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>39904</v>
       </c>
@@ -1773,20 +1510,17 @@
       <c r="C54">
         <v>40</v>
       </c>
-      <c r="F54">
-        <v>1.5359342915811101</v>
-      </c>
-      <c r="G54" t="s">
-        <v>9</v>
-      </c>
-      <c r="H54" t="s">
-        <v>12</v>
-      </c>
-      <c r="I54">
+      <c r="E54" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54">
         <v>79.099999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>39904</v>
       </c>
@@ -1796,20 +1530,17 @@
       <c r="C55">
         <v>40</v>
       </c>
-      <c r="F55">
-        <v>1.7084188911704301</v>
-      </c>
-      <c r="G55" t="s">
-        <v>9</v>
-      </c>
-      <c r="H55" t="s">
-        <v>12</v>
-      </c>
-      <c r="I55">
+      <c r="E55" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55">
         <v>78.2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>39904</v>
       </c>
@@ -1819,20 +1550,17 @@
       <c r="C56">
         <v>40</v>
       </c>
-      <c r="F56">
-        <v>1.9192334017796</v>
-      </c>
-      <c r="G56" t="s">
-        <v>9</v>
-      </c>
-      <c r="H56" t="s">
-        <v>12</v>
-      </c>
-      <c r="I56">
+      <c r="E56" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56">
         <v>78.900000000000006</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>39816</v>
       </c>
@@ -1842,20 +1570,17 @@
       <c r="C57">
         <v>40</v>
       </c>
-      <c r="F57">
-        <v>1.32785763175907</v>
-      </c>
-      <c r="G57" t="s">
-        <v>10</v>
-      </c>
-      <c r="H57" t="s">
-        <v>11</v>
-      </c>
-      <c r="I57">
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57">
         <v>12.2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>39816</v>
       </c>
@@ -1865,20 +1590,17 @@
       <c r="C58">
         <v>40</v>
       </c>
-      <c r="F58">
-        <v>1.9849418206707701</v>
-      </c>
-      <c r="G58" t="s">
-        <v>10</v>
-      </c>
-      <c r="H58" t="s">
-        <v>11</v>
-      </c>
-      <c r="I58">
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58">
         <v>13.8</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>39816</v>
       </c>
@@ -1888,20 +1610,17 @@
       <c r="C59">
         <v>40</v>
       </c>
-      <c r="F59">
-        <v>2.69130732375086</v>
-      </c>
-      <c r="G59" t="s">
-        <v>10</v>
-      </c>
-      <c r="H59" t="s">
-        <v>11</v>
-      </c>
-      <c r="I59">
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59">
         <v>12.5</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>39816</v>
       </c>
@@ -1911,20 +1630,17 @@
       <c r="C60">
         <v>40</v>
       </c>
-      <c r="F60">
-        <v>2.7460643394935</v>
-      </c>
-      <c r="G60" t="s">
-        <v>10</v>
-      </c>
-      <c r="H60" t="s">
-        <v>11</v>
-      </c>
-      <c r="I60">
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60">
         <v>12.5</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>39816</v>
       </c>
@@ -1934,20 +1650,17 @@
       <c r="C61">
         <v>40</v>
       </c>
-      <c r="F61">
-        <v>3.2443531827515399</v>
-      </c>
-      <c r="G61" t="s">
-        <v>10</v>
-      </c>
-      <c r="H61" t="s">
-        <v>11</v>
-      </c>
-      <c r="I61">
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61">
         <v>13.5</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>39816</v>
       </c>
@@ -1957,20 +1670,17 @@
       <c r="C62">
         <v>40</v>
       </c>
-      <c r="F62">
-        <v>3.4223134839151301</v>
-      </c>
-      <c r="G62" t="s">
-        <v>10</v>
-      </c>
-      <c r="H62" t="s">
-        <v>11</v>
-      </c>
-      <c r="I62">
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s">
+        <v>9</v>
+      </c>
+      <c r="G62">
         <v>14.3</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>39816</v>
       </c>
@@ -1980,20 +1690,17 @@
       <c r="C63">
         <v>40</v>
       </c>
-      <c r="F63">
-        <v>4.1642710472279303</v>
-      </c>
-      <c r="G63" t="s">
-        <v>10</v>
-      </c>
-      <c r="H63" t="s">
-        <v>11</v>
-      </c>
-      <c r="I63">
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63">
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>39816</v>
       </c>
@@ -2003,20 +1710,17 @@
       <c r="C64">
         <v>40</v>
       </c>
-      <c r="F64">
-        <v>4.8788501026694</v>
-      </c>
-      <c r="G64" t="s">
-        <v>10</v>
-      </c>
-      <c r="H64" t="s">
-        <v>11</v>
-      </c>
-      <c r="I64">
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64">
         <v>20.05</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>39816</v>
       </c>
@@ -2026,20 +1730,17 @@
       <c r="C65">
         <v>40</v>
       </c>
-      <c r="F65">
-        <v>4.9555099247090997</v>
-      </c>
-      <c r="G65" t="s">
-        <v>10</v>
-      </c>
-      <c r="H65" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65">
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65">
         <v>20.5</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>39816</v>
       </c>
@@ -2049,20 +1750,17 @@
       <c r="C66">
         <v>40</v>
       </c>
-      <c r="F66">
-        <v>5.0321697467488002</v>
-      </c>
-      <c r="G66" t="s">
-        <v>10</v>
-      </c>
-      <c r="H66" t="s">
-        <v>11</v>
-      </c>
-      <c r="I66">
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66">
         <v>19.850000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>39816</v>
       </c>
@@ -2072,20 +1770,17 @@
       <c r="C67">
         <v>40</v>
       </c>
-      <c r="F67">
-        <v>5.2785763175906899</v>
-      </c>
-      <c r="G67" t="s">
-        <v>10</v>
-      </c>
-      <c r="H67" t="s">
-        <v>11</v>
-      </c>
-      <c r="I67">
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67">
         <v>20.5</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>39816</v>
       </c>
@@ -2095,20 +1790,17 @@
       <c r="C68">
         <v>40</v>
       </c>
-      <c r="F68">
-        <v>5.7084188911704299</v>
-      </c>
-      <c r="G68" t="s">
-        <v>10</v>
-      </c>
-      <c r="H68" t="s">
-        <v>11</v>
-      </c>
-      <c r="I68">
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68">
         <v>21.9</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>39816</v>
       </c>
@@ -2118,20 +1810,17 @@
       <c r="C69">
         <v>40</v>
       </c>
-      <c r="F69">
-        <v>5.9356605065024004</v>
-      </c>
-      <c r="G69" t="s">
-        <v>10</v>
-      </c>
-      <c r="H69" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69">
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69">
         <v>22.8</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>39816</v>
       </c>
@@ -2141,20 +1830,17 @@
       <c r="C70">
         <v>40</v>
       </c>
-      <c r="F70">
-        <v>6.1273100616016398</v>
-      </c>
-      <c r="G70" t="s">
-        <v>10</v>
-      </c>
-      <c r="H70" t="s">
-        <v>11</v>
-      </c>
-      <c r="I70">
+      <c r="E70" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70">
         <v>22.3</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>39816</v>
       </c>
@@ -2164,20 +1850,17 @@
       <c r="C71">
         <v>40</v>
       </c>
-      <c r="F71">
-        <v>6.4120465434633802</v>
-      </c>
-      <c r="G71" t="s">
-        <v>10</v>
-      </c>
-      <c r="H71" t="s">
-        <v>11</v>
-      </c>
-      <c r="I71">
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71">
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>39816</v>
       </c>
@@ -2187,20 +1870,17 @@
       <c r="C72">
         <v>40</v>
       </c>
-      <c r="F72">
-        <v>1.32785763175907</v>
-      </c>
-      <c r="G72" t="s">
-        <v>10</v>
-      </c>
-      <c r="H72" t="s">
-        <v>12</v>
-      </c>
-      <c r="I72">
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72">
         <v>79.599999999999994</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>39816</v>
       </c>
@@ -2210,20 +1890,17 @@
       <c r="C73">
         <v>40</v>
       </c>
-      <c r="F73">
-        <v>2.69130732375086</v>
-      </c>
-      <c r="G73" t="s">
-        <v>10</v>
-      </c>
-      <c r="H73" t="s">
-        <v>12</v>
-      </c>
-      <c r="I73">
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" t="s">
+        <v>10</v>
+      </c>
+      <c r="G73">
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>39816</v>
       </c>
@@ -2233,20 +1910,17 @@
       <c r="C74">
         <v>40</v>
       </c>
-      <c r="F74">
-        <v>4.1642710472279303</v>
-      </c>
-      <c r="G74" t="s">
-        <v>10</v>
-      </c>
-      <c r="H74" t="s">
-        <v>12</v>
-      </c>
-      <c r="I74">
+      <c r="E74" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>39816</v>
       </c>
@@ -2256,20 +1930,17 @@
       <c r="C75">
         <v>40</v>
       </c>
-      <c r="F75">
-        <v>4.8788501026694</v>
-      </c>
-      <c r="G75" t="s">
-        <v>10</v>
-      </c>
-      <c r="H75" t="s">
-        <v>12</v>
-      </c>
-      <c r="I75">
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75">
         <v>102.7</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>39816</v>
       </c>
@@ -2279,20 +1950,17 @@
       <c r="C76">
         <v>40</v>
       </c>
-      <c r="F76">
-        <v>5.7084188911704299</v>
-      </c>
-      <c r="G76" t="s">
-        <v>10</v>
-      </c>
-      <c r="H76" t="s">
-        <v>12</v>
-      </c>
-      <c r="I76">
+      <c r="E76" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" t="s">
+        <v>10</v>
+      </c>
+      <c r="G76">
         <v>110</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>39816</v>
       </c>
@@ -2302,20 +1970,17 @@
       <c r="C77">
         <v>40</v>
       </c>
-      <c r="F77">
-        <v>5.9356605065024004</v>
-      </c>
-      <c r="G77" t="s">
-        <v>10</v>
-      </c>
-      <c r="H77" t="s">
-        <v>12</v>
-      </c>
-      <c r="I77">
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G77">
         <v>109.5</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>39816</v>
       </c>
@@ -2325,16 +1990,13 @@
       <c r="C78">
         <v>40</v>
       </c>
-      <c r="F78">
-        <v>6.1273100616016398</v>
-      </c>
-      <c r="G78" t="s">
-        <v>10</v>
-      </c>
-      <c r="H78" t="s">
-        <v>12</v>
-      </c>
-      <c r="I78">
+      <c r="E78" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" t="s">
+        <v>10</v>
+      </c>
+      <c r="G78">
         <v>109</v>
       </c>
     </row>

</xml_diff>